<commit_message>
updates with respo (temp correction, not with empty chambers yet
</commit_message>
<xml_diff>
--- a/log_slope_sections.xlsx
+++ b/log_slope_sections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristakraskura/Github_repositories/AR_KK_etal_MHWsim-corallimorph_respo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6247185-DE13-F643-8E38-47BA328CF31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AA049B-10B4-6046-AB61-AEDCE5105AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="27260" windowHeight="17500" xr2:uid="{0318DC34-714A-9E43-B6AC-BC84A5D37DF9}"/>
+    <workbookView xWindow="-34600" yWindow="2960" windowWidth="25080" windowHeight="17480" xr2:uid="{0318DC34-714A-9E43-B6AC-BC84A5D37DF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="125">
   <si>
     <t>Filename</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>Filename_plot</t>
+  </si>
+  <si>
+    <t>don’t use no back</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -511,21 +514,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,14 +871,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421EDBB7-25BD-8347-B193-176464C13436}">
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.1640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="75.6640625" style="11" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
     <col min="4" max="4" width="10.83203125" style="2"/>
     <col min="7" max="7" width="10.83203125" style="1"/>
@@ -880,44 +889,44 @@
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -926,7 +935,7 @@
         <f>SUBSTITUTE( B2, "_slopes.png", ".csv")</f>
         <v>2024-02-21_183903_022124_c1b13e2a5d9d8e14_tile_B_converted.csv</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1">
@@ -959,7 +968,7 @@
         <f t="shared" ref="A3:A66" si="0">SUBSTITUTE( B3, "_slopes.png", ".csv")</f>
         <v>2024-02-21_183903_022124_c1b13e2a5d9d8e14_tile_A_converted.csv</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1">
@@ -992,38 +1001,44 @@
         <f t="shared" si="0"/>
         <v>2024-02-21_150109_022124_c1b13e2a5d9d8e14_cory_B_converted.csv</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>50</v>
       </c>
       <c r="D4" s="2">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E4">
         <v>85</v>
       </c>
       <c r="F4">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G4" s="1">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H4" s="2">
-        <v>125</v>
+        <v>123</v>
+      </c>
+      <c r="I4" s="1">
+        <v>138</v>
+      </c>
+      <c r="J4" s="2">
+        <v>145</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K67" si="3">IF(ISBLANK(E4),1,(IF(ISBLANK(G4),2,IF(ISBLANK(I4),3,4))))</f>
-        <v>3</v>
+        <f t="shared" ref="K4:K68" si="3">IF(ISBLANK(E4),1,(IF(ISBLANK(G4),2,IF(ISBLANK(I4),3,4))))</f>
+        <v>4</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="1"/>
-        <v>50,85,115</v>
+        <v>50,85,113,138</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="2"/>
-        <v>70,95,125</v>
+        <v>64,93,123,145</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1031,38 +1046,44 @@
         <f t="shared" si="0"/>
         <v>2024-02-21_150109_022124_c1b13e2a5d9d8e14_cory_A_converted.csv</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="1">
         <v>50</v>
       </c>
       <c r="D5" s="2">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E5">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G5" s="1">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H5" s="2">
-        <v>125</v>
+        <v>121</v>
+      </c>
+      <c r="I5" s="1">
+        <v>138</v>
+      </c>
+      <c r="J5" s="2">
+        <v>145</v>
       </c>
       <c r="K5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="1"/>
-        <v>50,85,115</v>
+        <v>50,84,111,138</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="2"/>
-        <v>70,95,125</v>
+        <v>64,92,121,145</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1070,14 +1091,14 @@
         <f t="shared" si="0"/>
         <v>2024-02-21_133047_022124_AMB_810610796_tile_B_converted.csv</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="1">
         <v>53</v>
       </c>
       <c r="D6" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
@@ -1089,7 +1110,7 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1097,7 +1118,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-21_133047_022124_AMB_810610796_tile_A_converted.csv</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="1">
@@ -1124,7 +1145,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-21_100008_022124_AMB_810610796_cory_B_converted.csv</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1">
@@ -1140,16 +1161,16 @@
         <v>83</v>
       </c>
       <c r="G8" s="1">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H8" s="2">
         <v>111</v>
       </c>
       <c r="I8" s="1">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J8" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K8">
         <f t="shared" si="3"/>
@@ -1157,11 +1178,11 @@
       </c>
       <c r="L8" t="str">
         <f t="shared" si="1"/>
-        <v>50,75,101,134</v>
+        <v>50,75,102,136</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="2"/>
-        <v>60,83,111,144</v>
+        <v>60,83,111,145</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1169,7 +1190,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-21_100008_022124_AMB_810610796_cory_A_converted.csv</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="1">
@@ -1214,7 +1235,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-20_174924_022024_PME_11151214121513_tile_B_converted.csv</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="1">
@@ -1224,7 +1245,7 @@
         <v>51</v>
       </c>
       <c r="E10">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F10">
         <v>80</v>
@@ -1235,7 +1256,7 @@
       </c>
       <c r="L10" t="str">
         <f t="shared" si="1"/>
-        <v>43,70</v>
+        <v>43,71</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="2"/>
@@ -1247,7 +1268,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-20_174924_022024_PME_11151214121513_tile_A_converted.csv</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="1">
@@ -1280,7 +1301,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-20_141318_022024_PME_11151214121513_cory_B_converted.csv</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="1">
@@ -1290,16 +1311,16 @@
         <v>50</v>
       </c>
       <c r="E12">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F12">
         <v>78</v>
       </c>
       <c r="G12" s="1">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H12" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I12" s="1">
         <v>135</v>
@@ -1313,11 +1334,11 @@
       </c>
       <c r="L12" t="str">
         <f t="shared" si="1"/>
-        <v>40,69,105,135</v>
+        <v>40,70,104,135</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="2"/>
-        <v>50,78,113,142</v>
+        <v>50,78,112,142</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1325,7 +1346,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-20_141318_022024_PME_11151214121513_cory_A_converted.csv</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="1">
@@ -1347,10 +1368,10 @@
         <v>110</v>
       </c>
       <c r="I13" s="1">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J13" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
@@ -1358,11 +1379,11 @@
       </c>
       <c r="L13" t="str">
         <f t="shared" si="1"/>
-        <v>40,69,100,132</v>
+        <v>40,69,100,133</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="2"/>
-        <v>48,76,110,141</v>
+        <v>48,76,110,142</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1370,7 +1391,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-20_125557_022024_AMA_1142345_tile_B_converted.csv</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="1">
@@ -1397,7 +1418,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-20_125557_022024_AMA_1142345_tile_A_converted.csv</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="1">
@@ -1424,7 +1445,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-20_092644_022024_AMA_1142345_cory_B_converted.csv</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="1">
@@ -1469,7 +1490,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-20_092644_022024_AMA_1142345_cory_A_converted.csv</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="1">
@@ -1514,7 +1535,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-19_183927_021924_PME_2153541_tile_B_converted.csv</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="1">
@@ -1553,7 +1574,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-19_183927_021924_PME_2153541_tile_A_converted.csv</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="1">
@@ -1592,7 +1613,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-19_145106_021924_PME_2153541_cory_B_converted.csv</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="1">
@@ -1605,7 +1626,7 @@
         <v>67</v>
       </c>
       <c r="F20">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G20" s="1">
         <v>95</v>
@@ -1629,7 +1650,7 @@
       </c>
       <c r="M20" t="str">
         <f t="shared" si="2"/>
-        <v>48,77,103,135</v>
+        <v>48,76,103,135</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1637,7 +1658,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-19_145106_021924_PME_2153541_cory_A_converted.csv</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="1">
@@ -1682,7 +1703,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-19_131005_021924_AMB_2531543_tile_B_converted.csv</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="1">
@@ -1715,7 +1736,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-19_131005_021924_AMB_2531543_tile_A_converted.csv</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="3">
@@ -1748,7 +1769,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-19_093616_021924_AMB_2531543_cory_B_converted.csv</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="1">
@@ -1793,7 +1814,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-19_093616_021924_AMB_2531543_cory_A_converted.csv</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="1">
@@ -1803,10 +1824,10 @@
         <v>52</v>
       </c>
       <c r="E25">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F25">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G25" s="1">
         <v>92</v>
@@ -1826,11 +1847,11 @@
       </c>
       <c r="L25" t="str">
         <f t="shared" si="1"/>
-        <v>45,69,92,119</v>
+        <v>45,70,92,119</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="2"/>
-        <v>52,77,101,127</v>
+        <v>52,78,101,127</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -1838,7 +1859,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-18_191728_021824_PMD_13121311151412_tile_B_converted.csv</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="1">
@@ -1871,7 +1892,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-18_191728_021824_PMD_13121311151412_tile_A_converted.csv</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="1">
@@ -1904,7 +1925,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-18_154443_021824_PMD_13121311151412_cory_B_converted.csv</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C28" s="1">
@@ -1949,7 +1970,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-18_154443_021824_PMD_13121311151412_cory_A_converted.csv</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="1">
@@ -1971,7 +1992,7 @@
         <v>130</v>
       </c>
       <c r="I29" s="1">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J29" s="2">
         <v>159</v>
@@ -1982,7 +2003,7 @@
       </c>
       <c r="L29" t="str">
         <f t="shared" si="1"/>
-        <v>41,91,121,149</v>
+        <v>41,91,121,151</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="2"/>
@@ -1994,7 +2015,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-18_140427_021824_AMB_12141214151311_tile_B_converted.csv</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C30" s="1">
@@ -2009,17 +2030,23 @@
       <c r="F30">
         <v>63</v>
       </c>
+      <c r="G30" s="1">
+        <v>84</v>
+      </c>
+      <c r="H30" s="2">
+        <v>90</v>
+      </c>
       <c r="K30">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="1"/>
-        <v>30.5,54</v>
+        <v>30.5,54,84</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="2"/>
-        <v>38,63</v>
+        <v>38,63,90</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -2027,7 +2054,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-18_140427_021824_AMB_12141214151311_tile_A_converted.csv</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="1">
@@ -2060,7 +2087,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-18_102803_021824_AMB_12141214151311_cory_B_converted.csv</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="1">
@@ -2076,10 +2103,10 @@
         <v>85</v>
       </c>
       <c r="G32" s="1">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H32" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I32" s="1">
         <v>134</v>
@@ -2093,11 +2120,11 @@
       </c>
       <c r="L32" t="str">
         <f t="shared" si="1"/>
-        <v>45,76,104,134</v>
+        <v>45,76,105,134</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" si="2"/>
-        <v>55,85,114,145</v>
+        <v>55,85,115,145</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -2105,7 +2132,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-18_102803_021824_AMB_12141214151311_cory_A_converted.csv</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C33" s="1">
@@ -2121,10 +2148,10 @@
         <v>85</v>
       </c>
       <c r="G33" s="1">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H33" s="2">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I33" s="1">
         <v>132</v>
@@ -2138,11 +2165,11 @@
       </c>
       <c r="L33" t="str">
         <f t="shared" si="1"/>
-        <v>45,74,101,132</v>
+        <v>45,74,103,132</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="2"/>
-        <v>52,85,110,141</v>
+        <v>52,85,102,141</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -2150,14 +2177,14 @@
         <f t="shared" si="0"/>
         <v>2024-02-17_175800_021724_PME_87610697_tile_B_converted.csv</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="11" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="1">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D34" s="2">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K34">
         <f t="shared" si="3"/>
@@ -2165,11 +2192,11 @@
       </c>
       <c r="L34" t="str">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="2"/>
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -2177,7 +2204,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-17_175800_021724_PME_87610697_tile_A_converted.csv</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="1">
@@ -2204,20 +2231,20 @@
         <f t="shared" si="0"/>
         <v>2024-02-17_143425_021724_PME_87610697_cory_B_converted.csv</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C36" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D36" s="2">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E36">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F36">
-        <v>81</v>
+        <v>82.5</v>
       </c>
       <c r="G36" s="1">
         <v>99</v>
@@ -2237,11 +2264,11 @@
       </c>
       <c r="L36" t="str">
         <f t="shared" si="1"/>
-        <v>41,72,99,121</v>
+        <v>42,73,99,121</v>
       </c>
       <c r="M36" t="str">
         <f t="shared" si="2"/>
-        <v>50,81,106,130</v>
+        <v>52,82.5,106,130</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -2249,7 +2276,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-17_143425_021724_PME_87610697_cory_A_converted.csv</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C37" s="1">
@@ -2259,16 +2286,16 @@
         <v>50</v>
       </c>
       <c r="E37">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F37">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G37" s="1">
         <v>97</v>
       </c>
       <c r="H37" s="2">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I37" s="1">
         <v>119</v>
@@ -2282,11 +2309,11 @@
       </c>
       <c r="L37" t="str">
         <f t="shared" si="1"/>
-        <v>41,70,97,119</v>
+        <v>41,71,97,119</v>
       </c>
       <c r="M37" t="str">
         <f t="shared" si="2"/>
-        <v>50,80,105,126</v>
+        <v>50,81,104,126</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -2294,7 +2321,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-17_124743_021724_AMA_60787109_tile_B_converted.csv</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C38" s="1">
@@ -2327,7 +2354,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-17_124743_021724_AMA_60787109_tile_A_converted.csv</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C39" s="1">
@@ -2366,7 +2393,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-17_091905_021724_AMA_60787109_cory_B_converted.csv</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="11" t="s">
         <v>49</v>
       </c>
       <c r="C40" s="1">
@@ -2411,7 +2438,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-17_091905_021724_AMA_60787109_cory_A_converted.csv</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C41" s="1">
@@ -2427,7 +2454,7 @@
         <v>90</v>
       </c>
       <c r="G41" s="1">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="H41" s="2">
         <v>118</v>
@@ -2444,7 +2471,7 @@
       </c>
       <c r="L41" t="str">
         <f t="shared" si="1"/>
-        <v>51,81,101,136</v>
+        <v>51,81,111,136</v>
       </c>
       <c r="M41" t="str">
         <f t="shared" si="2"/>
@@ -2456,7 +2483,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-16_184833_021624_PMD_3451215_tile_B_converted.csv</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="11" t="s">
         <v>51</v>
       </c>
       <c r="C42" s="1">
@@ -2471,17 +2498,23 @@
       <c r="F42">
         <v>80</v>
       </c>
+      <c r="G42" s="1">
+        <v>92</v>
+      </c>
+      <c r="H42" s="2">
+        <v>97</v>
+      </c>
       <c r="K42">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" si="1"/>
-        <v>52,73</v>
+        <v>52,73,92</v>
       </c>
       <c r="M42" t="str">
         <f t="shared" si="2"/>
-        <v>60,80</v>
+        <v>60,80,97</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -2489,32 +2522,38 @@
         <f t="shared" si="0"/>
         <v>2024-02-16_184833_021624_PMD_3451215_tile_A_converted.csv</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C43" s="1">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D43" s="2">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E43">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F43">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="G43" s="1">
+        <v>92</v>
+      </c>
+      <c r="H43" s="2">
+        <v>97</v>
       </c>
       <c r="K43">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" si="1"/>
-        <v>48,70</v>
+        <v>51,72,92</v>
       </c>
       <c r="M43" t="str">
         <f t="shared" si="2"/>
-        <v>58,77</v>
+        <v>60,78,97</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
@@ -2522,26 +2561,26 @@
         <f t="shared" si="0"/>
         <v>2024-02-16_150056_021624_PMD_3451215_cory_B_converted.csv</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C44" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D44" s="2">
         <v>65</v>
       </c>
       <c r="E44">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F44">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G44" s="1">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H44" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K44">
         <f t="shared" si="3"/>
@@ -2549,11 +2588,11 @@
       </c>
       <c r="L44" t="str">
         <f t="shared" si="1"/>
-        <v>53,98,127</v>
+        <v>54,99,129</v>
       </c>
       <c r="M44" t="str">
         <f t="shared" si="2"/>
-        <v>65,108,138</v>
+        <v>65,109,139</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -2561,14 +2600,14 @@
         <f t="shared" si="0"/>
         <v>2024-02-16_150056_021624_PMD_3451215_cory_A_converted.csv</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C45" s="1">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D45" s="2">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E45">
         <v>74</v>
@@ -2583,10 +2622,10 @@
         <v>106</v>
       </c>
       <c r="I45" s="1">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J45" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K45">
         <f t="shared" si="3"/>
@@ -2594,11 +2633,11 @@
       </c>
       <c r="L45" t="str">
         <f t="shared" si="1"/>
-        <v>52,74,98,128</v>
+        <v>54,74,98,129</v>
       </c>
       <c r="M45" t="str">
         <f t="shared" si="2"/>
-        <v>62,81,106,136</v>
+        <v>64,81,106,137</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -2606,7 +2645,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-16_130931_021624_AMA_15111214131112_tile_B_converted.csv</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="11" t="s">
         <v>55</v>
       </c>
       <c r="C46" s="1">
@@ -2639,7 +2678,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-16_130931_021624_AMA_15111214131112_tile_A_converted.csv</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C47" s="1">
@@ -2672,7 +2711,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-16_093548_021624_AMA_15111214131112_cory_B_converted.csv</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="11" t="s">
         <v>57</v>
       </c>
       <c r="C48" s="1">
@@ -2694,10 +2733,10 @@
         <v>96</v>
       </c>
       <c r="I48" s="1">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J48" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K48">
         <f t="shared" si="3"/>
@@ -2705,11 +2744,11 @@
       </c>
       <c r="L48" t="str">
         <f t="shared" si="1"/>
-        <v>42,60,87,118</v>
+        <v>42,60,87,119</v>
       </c>
       <c r="M48" t="str">
         <f t="shared" si="2"/>
-        <v>49,69,96,128</v>
+        <v>49,69,96,127</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
@@ -2717,7 +2756,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-16_093548_021624_AMA_15111214131112_cory_A_converted.csv</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C49" s="1">
@@ -2733,16 +2772,16 @@
         <v>67</v>
       </c>
       <c r="G49" s="1">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H49" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I49" s="1">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J49" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K49">
         <f t="shared" si="3"/>
@@ -2750,11 +2789,11 @@
       </c>
       <c r="L49" t="str">
         <f t="shared" si="1"/>
-        <v>41,60,86,118</v>
+        <v>41,60,87,119</v>
       </c>
       <c r="M49" t="str">
         <f t="shared" si="2"/>
-        <v>48,67,93,125</v>
+        <v>48,67,94,126</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -2762,7 +2801,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-15_173144_021524_PMC_2354135_tile_B_converted.csv</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C50" s="1">
@@ -2775,7 +2814,7 @@
         <v>71</v>
       </c>
       <c r="F50">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K50">
         <f t="shared" si="3"/>
@@ -2787,7 +2826,7 @@
       </c>
       <c r="M50" t="str">
         <f t="shared" si="2"/>
-        <v>51,80</v>
+        <v>51,79</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
@@ -2795,7 +2834,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-15_173144_021524_PMC_2354135_tile_A_converted.csv</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C51" s="1">
@@ -2808,7 +2847,7 @@
         <v>69</v>
       </c>
       <c r="F51">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K51">
         <f t="shared" si="3"/>
@@ -2820,7 +2859,7 @@
       </c>
       <c r="M51" t="str">
         <f t="shared" si="2"/>
-        <v>50,80</v>
+        <v>50,79</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
@@ -2828,7 +2867,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-15_135208_021524_PMC_2354135_cory_B_converted.csv</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="11" t="s">
         <v>61</v>
       </c>
       <c r="C52" s="4">
@@ -2844,13 +2883,13 @@
         <v>73</v>
       </c>
       <c r="G52" s="1">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H52" s="2">
         <v>105</v>
       </c>
       <c r="I52" s="1">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J52" s="2">
         <v>135</v>
@@ -2861,7 +2900,7 @@
       </c>
       <c r="L52" t="str">
         <f t="shared" si="1"/>
-        <v>35,64,95,127</v>
+        <v>35,64,96,128</v>
       </c>
       <c r="M52" t="str">
         <f t="shared" si="2"/>
@@ -2873,20 +2912,20 @@
         <f t="shared" si="0"/>
         <v>2024-02-15_135208_021524_PMC_2354135_cory_A_converted.csv</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C53" s="1">
         <v>35</v>
       </c>
       <c r="D53" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E53">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F53">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G53" s="1">
         <v>97</v>
@@ -2906,11 +2945,11 @@
       </c>
       <c r="L53" t="str">
         <f t="shared" si="1"/>
-        <v>35,62,97,152</v>
+        <v>35,63,97,152</v>
       </c>
       <c r="M53" t="str">
         <f t="shared" si="2"/>
-        <v>45,71,105,159</v>
+        <v>44,72,105,159</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
@@ -2918,20 +2957,20 @@
         <f t="shared" si="0"/>
         <v>2024-02-15_120433_021524_AMC_11111414131215_tile_B_converted.csv</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C54" s="1">
-        <v>40</v>
+        <v>40.5</v>
       </c>
       <c r="D54" s="2">
-        <v>46</v>
+        <v>46.5</v>
       </c>
       <c r="E54">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F54">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K54">
         <f t="shared" si="3"/>
@@ -2939,11 +2978,11 @@
       </c>
       <c r="L54" t="str">
         <f t="shared" si="1"/>
-        <v>40,66</v>
+        <v>40.5,67</v>
       </c>
       <c r="M54" t="str">
         <f t="shared" si="2"/>
-        <v>46,75</v>
+        <v>46.5,77</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -2951,7 +2990,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-15_120433_021524_AMC_11111414131215_tile_A_converted.csv</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="11" t="s">
         <v>64</v>
       </c>
       <c r="C55" s="1">
@@ -2984,7 +3023,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-15_092912_2024-02-15_AMC_11111414131215_cory_B_converted.csv</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="11" t="s">
         <v>65</v>
       </c>
       <c r="C56" s="1">
@@ -2994,13 +3033,13 @@
         <v>38</v>
       </c>
       <c r="E56">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F56">
         <v>66</v>
       </c>
       <c r="G56" s="1">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H56" s="2">
         <v>95</v>
@@ -3009,7 +3048,7 @@
         <v>111</v>
       </c>
       <c r="J56" s="2">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K56">
         <f t="shared" si="3"/>
@@ -3017,11 +3056,11 @@
       </c>
       <c r="L56" t="str">
         <f t="shared" si="1"/>
-        <v>30.5,59,85,111</v>
+        <v>30.5,58,86,111</v>
       </c>
       <c r="M56" t="str">
         <f t="shared" si="2"/>
-        <v>38,66,95,120</v>
+        <v>38,66,95,119</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
@@ -3029,7 +3068,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-15_092912_2024-02-15_AMC_11111414131215_cory_A_converted.csv</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="11" t="s">
         <v>66</v>
       </c>
       <c r="C57" s="1">
@@ -3054,7 +3093,7 @@
         <v>112</v>
       </c>
       <c r="J57" s="2">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K57">
         <f t="shared" si="3"/>
@@ -3066,7 +3105,7 @@
       </c>
       <c r="M57" t="str">
         <f t="shared" si="2"/>
-        <v>38,66,95,120</v>
+        <v>38,66,95,119</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -3074,14 +3113,14 @@
         <f t="shared" si="0"/>
         <v>2024-02-14_194709_2024-02-14_PMC_791010689_tile_B_converted.csv</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C58" s="1">
         <v>30.5</v>
       </c>
       <c r="D58" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E58">
         <v>55</v>
@@ -3099,7 +3138,7 @@
       </c>
       <c r="M58" t="str">
         <f t="shared" si="2"/>
-        <v>39,64</v>
+        <v>38,64</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
@@ -3107,7 +3146,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-14_194709_2024-02-14_PMC_791010689_tile_A_converted.csv</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C59" s="1">
@@ -3140,7 +3179,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-14_161244_2024-02-14_PMC_791010689_cory_B_converted.csv</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C60" s="1">
@@ -3185,7 +3224,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-14_161244_2024-02-14_PMC_791010689_cory_A_converted.csv</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="11" t="s">
         <v>70</v>
       </c>
       <c r="C61" s="1">
@@ -3230,7 +3269,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-14_143551_2024-02-14_AMD_98976108_tile_B_converted.csv</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C62" s="1">
@@ -3240,7 +3279,7 @@
         <v>39</v>
       </c>
       <c r="E62">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F62">
         <v>65</v>
@@ -3251,7 +3290,7 @@
       </c>
       <c r="L62" t="str">
         <f t="shared" si="1"/>
-        <v>31,55</v>
+        <v>31,56</v>
       </c>
       <c r="M62" t="str">
         <f t="shared" si="2"/>
@@ -3263,7 +3302,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-14_143551_2024-02-14_AMD_98976108_tile_A_converted.csv</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="11" t="s">
         <v>72</v>
       </c>
       <c r="C63" s="1">
@@ -3296,14 +3335,14 @@
         <f t="shared" si="0"/>
         <v>2024-02-14_104544_2024-02-14_AMD_98976108_cory_B_converted.csv</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C64" s="1">
         <v>55</v>
       </c>
       <c r="D64" s="2">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E64">
         <v>80</v>
@@ -3333,7 +3372,7 @@
       </c>
       <c r="M64" t="str">
         <f t="shared" si="2"/>
-        <v>65,90,115,138</v>
+        <v>64,90,115,138</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
@@ -3341,7 +3380,7 @@
         <f t="shared" si="0"/>
         <v>2024-02-14_104544_2024-02-14_AMD_98976108_cory_A_converted.csv</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="11" t="s">
         <v>74</v>
       </c>
       <c r="C65" s="1">
@@ -3354,7 +3393,7 @@
         <v>79</v>
       </c>
       <c r="F65">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G65" s="1">
         <v>105</v>
@@ -3378,7 +3417,7 @@
       </c>
       <c r="M65" t="str">
         <f t="shared" si="2"/>
-        <v>61,88,113,136</v>
+        <v>61,87,113,136</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
@@ -3386,14 +3425,14 @@
         <f t="shared" si="0"/>
         <v>2023-12-12_215441_121223_15C_A2B2E2B3E3A4_tile_B_converted.csv</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C66" s="1">
         <v>30.5</v>
       </c>
       <c r="D66" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E66">
         <v>59</v>
@@ -3408,10 +3447,10 @@
         <v>97</v>
       </c>
       <c r="I66" s="1">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J66" s="2">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K66">
         <f t="shared" si="3"/>
@@ -3419,11 +3458,11 @@
       </c>
       <c r="L66" t="str">
         <f t="shared" si="1"/>
-        <v>30.5,59,89,116</v>
+        <v>30.5,59,89,118</v>
       </c>
       <c r="M66" t="str">
         <f t="shared" si="2"/>
-        <v>40,68,97,125</v>
+        <v>39,68,97,123</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
@@ -3431,7 +3470,7 @@
         <f t="shared" ref="A67:A111" si="4">SUBSTITUTE( B67, "_slopes.png", ".csv")</f>
         <v>2023-12-12_215441_121223_15C_A2B2E2B3E3A4_tile_A_converted.csv</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="11" t="s">
         <v>76</v>
       </c>
       <c r="C67" s="1">
@@ -3444,7 +3483,7 @@
         <v>59</v>
       </c>
       <c r="F67">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G67" s="1">
         <v>87</v>
@@ -3453,10 +3492,10 @@
         <v>95</v>
       </c>
       <c r="I67" s="1">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J67" s="2">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K67">
         <f t="shared" si="3"/>
@@ -3464,11 +3503,11 @@
       </c>
       <c r="L67" t="str">
         <f t="shared" ref="L67:L111" si="5">IF($K67=1,_xlfn.CONCAT(C67),IF($K67=2,_xlfn.CONCAT(,C67,",",E67),IF($K67=3,_xlfn.CONCAT(C67,",",E67,",",G67),_xlfn.CONCAT(C67,",",E67,",",G67,",",I67))))</f>
-        <v>30.5,59,87,116</v>
+        <v>30.5,59,87,118</v>
       </c>
       <c r="M67" t="str">
         <f t="shared" ref="M67:M111" si="6">IF($K67=1,_xlfn.CONCAT(D67),IF($K67=2,_xlfn.CONCAT(,D67,",",F67),IF($K67=3,_xlfn.CONCAT(D67,",",F67,",",H67),_xlfn.CONCAT(D67,",",F67,",",H67,",",J67))))</f>
-        <v>38,68,95,125</v>
+        <v>38,67,95,123</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
@@ -3476,44 +3515,38 @@
         <f t="shared" si="4"/>
         <v>2023-12-12_182021_121223_15C_A2B2E2B3E3A4_cory_B_converted.csv</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="11" t="s">
         <v>77</v>
       </c>
       <c r="C68" s="1">
-        <v>30.5</v>
+        <v>80</v>
       </c>
       <c r="D68" s="2">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E68">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="F68">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="G68" s="1">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="H68" s="2">
-        <v>101</v>
-      </c>
-      <c r="I68" s="1">
-        <v>125</v>
-      </c>
-      <c r="J68" s="2">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K68">
-        <f t="shared" ref="K68:K111" si="7">IF(ISBLANK(E68),1,(IF(ISBLANK(G68),2,IF(ISBLANK(I68),3,4))))</f>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>3</v>
       </c>
       <c r="L68" t="str">
         <f t="shared" si="5"/>
-        <v>30.5,62,91,125</v>
+        <v>80,94,124</v>
       </c>
       <c r="M68" t="str">
         <f t="shared" si="6"/>
-        <v>45,71,101,133</v>
+        <v>90,101,132</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
@@ -3521,7 +3554,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-12_182021_121223_15C_A2B2E2B3E3A4_cory_A_converted.csv</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C69" s="1">
@@ -3549,7 +3582,7 @@
         <v>135</v>
       </c>
       <c r="K69">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="K69:K111" si="7">IF(ISBLANK(E69),1,(IF(ISBLANK(G69),2,IF(ISBLANK(I69),3,4))))</f>
         <v>4</v>
       </c>
       <c r="L69" t="str">
@@ -3566,7 +3599,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-12_144729_121123_15C_A7B7E7A8B9E10_tile_B_converted.csv</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="11" t="s">
         <v>79</v>
       </c>
       <c r="C70" s="1">
@@ -3599,7 +3632,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-12_144729_121123_15C_A7B7E7A8B9E10_tile_A_converted.csv</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="11" t="s">
         <v>80</v>
       </c>
       <c r="C71" s="1">
@@ -3632,7 +3665,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-12_110637_121123_15C_A7B7E7A8B9E10_cory_B_converted.csv</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="11" t="s">
         <v>81</v>
       </c>
       <c r="C72" s="1">
@@ -3677,7 +3710,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-12_110637_121123_15C_A7B7E7A8B9E10_cory_A_converted.csv</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="11" t="s">
         <v>82</v>
       </c>
       <c r="C73" s="1">
@@ -3722,7 +3755,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-11_171114_121123_23C_B11A14E14B14A15E15_tile_B_converted.csv</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C74" s="1">
@@ -3767,7 +3800,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-11_171114_121123_23C_B11A14E14B14A15E15_tile_A_converted.csv</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="11" t="s">
         <v>84</v>
       </c>
       <c r="C75" s="1">
@@ -3812,44 +3845,38 @@
         <f t="shared" si="4"/>
         <v>2023-12-11_132532_121123_23C_B11A14E14B14A15E15_cory_B_converted.csv</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C76" s="1">
-        <v>30.5</v>
-      </c>
-      <c r="D76" s="2">
-        <v>45</v>
-      </c>
-      <c r="E76">
+      <c r="C76">
         <v>85</v>
       </c>
-      <c r="F76">
+      <c r="D76">
         <v>100</v>
       </c>
+      <c r="E76" s="1">
+        <v>105</v>
+      </c>
+      <c r="F76" s="2">
+        <v>120</v>
+      </c>
       <c r="G76" s="1">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="H76" s="2">
-        <v>120</v>
-      </c>
-      <c r="I76" s="1">
-        <v>123</v>
-      </c>
-      <c r="J76" s="2">
         <v>140</v>
       </c>
       <c r="K76">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="L76" t="str">
-        <f t="shared" si="5"/>
-        <v>30.5,85,105,123</v>
-      </c>
-      <c r="M76" t="str">
-        <f t="shared" si="6"/>
-        <v>45,100,120,140</v>
+        <f>IF(ISBLANK(C76),1,(IF(ISBLANK(E76),2,IF(ISBLANK(G76),3,4))))</f>
+        <v>4</v>
+      </c>
+      <c r="L76" t="e">
+        <f>IF($K76=1,_xlfn.CONCAT(#REF!),IF($K76=2,_xlfn.CONCAT(,#REF!,",",C76),IF($K76=3,_xlfn.CONCAT(#REF!,",",C76,",",E76),_xlfn.CONCAT(#REF!,",",C76,",",E76,",",G76))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M76" t="e">
+        <f>IF($K76=1,_xlfn.CONCAT(#REF!),IF($K76=2,_xlfn.CONCAT(,#REF!,",",D76),IF($K76=3,_xlfn.CONCAT(#REF!,",",D76,",",F76),_xlfn.CONCAT(#REF!,",",D76,",",F76,",",H76))))</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
@@ -3857,44 +3884,38 @@
         <f t="shared" si="4"/>
         <v>2023-12-11_132532_121123_23C_B11A14E14B14A15E15_cory_A_converted.csv</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C77" s="1">
-        <v>30.5</v>
-      </c>
-      <c r="D77" s="2">
-        <v>45</v>
-      </c>
-      <c r="E77">
+      <c r="C77">
         <v>85</v>
       </c>
-      <c r="F77">
+      <c r="D77">
         <v>100</v>
       </c>
+      <c r="E77" s="1">
+        <v>105</v>
+      </c>
+      <c r="F77" s="2">
+        <v>120</v>
+      </c>
       <c r="G77" s="1">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="H77" s="2">
-        <v>120</v>
-      </c>
-      <c r="I77" s="1">
-        <v>123</v>
-      </c>
-      <c r="J77" s="2">
         <v>140</v>
       </c>
       <c r="K77">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="L77" t="str">
-        <f t="shared" si="5"/>
-        <v>30.5,85,105,123</v>
-      </c>
-      <c r="M77" t="str">
-        <f t="shared" si="6"/>
-        <v>45,100,120,140</v>
+        <f>IF(ISBLANK(C77),1,(IF(ISBLANK(E77),2,IF(ISBLANK(G77),3,4))))</f>
+        <v>4</v>
+      </c>
+      <c r="L77" t="e">
+        <f>IF($K77=1,_xlfn.CONCAT(#REF!),IF($K77=2,_xlfn.CONCAT(,#REF!,",",C77),IF($K77=3,_xlfn.CONCAT(#REF!,",",C77,",",E77),_xlfn.CONCAT(#REF!,",",C77,",",E77,",",G77))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M77" t="e">
+        <f>IF($K77=1,_xlfn.CONCAT(#REF!),IF($K77=2,_xlfn.CONCAT(,#REF!,",",D77),IF($K77=3,_xlfn.CONCAT(#REF!,",",D77,",",F77),_xlfn.CONCAT(#REF!,",",D77,",",F77,",",H77))))</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
@@ -3902,7 +3923,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-10_193218_121023_15C_B1A2A3_tile_A_converted.csv</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="11" t="s">
         <v>87</v>
       </c>
       <c r="C78" s="1">
@@ -3941,7 +3962,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-10_160604_121023_15C_B1A2A3_cory_A_converted.csv</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="11" t="s">
         <v>88</v>
       </c>
       <c r="C79" s="1">
@@ -3954,19 +3975,19 @@
         <v>65</v>
       </c>
       <c r="F79">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G79" s="1">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H79" s="2">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I79" s="1">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J79" s="2">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K79">
         <f t="shared" si="7"/>
@@ -3974,11 +3995,11 @@
       </c>
       <c r="L79" t="str">
         <f t="shared" si="5"/>
-        <v>36,65,95,123</v>
+        <v>36,65,94,122</v>
       </c>
       <c r="M79" t="str">
         <f t="shared" si="6"/>
-        <v>45,75,103,130</v>
+        <v>45,74,102,129</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
@@ -3986,7 +4007,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-10_144051_121023_15C_E1E2E4E3E4E5_tile_B_converted.csv</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="11" t="s">
         <v>89</v>
       </c>
       <c r="C80" s="1">
@@ -4019,7 +4040,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-10_144051_121023_15C_E1E2E4E3E4E5_tile_A_converted.csv</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="11" t="s">
         <v>90</v>
       </c>
       <c r="C81" s="1">
@@ -4032,13 +4053,13 @@
         <v>52</v>
       </c>
       <c r="F81">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G81" s="1">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H81" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K81">
         <f t="shared" si="7"/>
@@ -4046,11 +4067,11 @@
       </c>
       <c r="L81" t="str">
         <f t="shared" si="5"/>
-        <v>31,52,70</v>
+        <v>31,52,71</v>
       </c>
       <c r="M81" t="str">
         <f t="shared" si="6"/>
-        <v>40,60,76</v>
+        <v>40,59,77</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -4058,7 +4079,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-10_110928_121023_15C_E1E2E4E3E4E5_cory_B_converted.csv</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="11" t="s">
         <v>91</v>
       </c>
       <c r="C82" s="1">
@@ -4068,10 +4089,10 @@
         <v>50</v>
       </c>
       <c r="E82">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F82">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G82" s="1">
         <v>98</v>
@@ -4091,11 +4112,11 @@
       </c>
       <c r="L82" t="str">
         <f t="shared" si="5"/>
-        <v>40,70,98,145</v>
+        <v>40,69,98,145</v>
       </c>
       <c r="M82" t="str">
         <f t="shared" si="6"/>
-        <v>50,80,104,150</v>
+        <v>50,79,104,150</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -4103,7 +4124,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-10_110928_121023_15C_E1E2E4E3E4E5_cory_A_converted.csv</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="11" t="s">
         <v>92</v>
       </c>
       <c r="C83" s="1">
@@ -4122,7 +4143,7 @@
         <v>96</v>
       </c>
       <c r="H83" s="2">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I83" s="1">
         <v>119</v>
@@ -4140,7 +4161,7 @@
       </c>
       <c r="M83" t="str">
         <f t="shared" si="6"/>
-        <v>46,77,105,127</v>
+        <v>46,77,104,127</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
@@ -4148,7 +4169,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-09_160745_120923_15C_A1B1A4B4A5B5_tile_B_converted.csv</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="11" t="s">
         <v>93</v>
       </c>
       <c r="C84" s="1">
@@ -4181,7 +4202,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-09_160745_120923_15C_A1B1A4B4A5B5_tile_A_converted.csv</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="11" t="s">
         <v>94</v>
       </c>
       <c r="C85" s="1">
@@ -4191,10 +4212,10 @@
         <v>58</v>
       </c>
       <c r="E85">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F85">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K85">
         <f t="shared" si="7"/>
@@ -4202,11 +4223,11 @@
       </c>
       <c r="L85" t="str">
         <f t="shared" si="5"/>
-        <v>48,80</v>
+        <v>48,79</v>
       </c>
       <c r="M85" t="str">
         <f t="shared" si="6"/>
-        <v>58,90</v>
+        <v>58,87</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -4214,26 +4235,26 @@
         <f t="shared" si="4"/>
         <v>2023-12-09_122228_120923_15C_A1B1A4B4A5B5_cory_B_converted.csv</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="11" t="s">
         <v>95</v>
       </c>
       <c r="C86" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D86" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E86">
         <v>80</v>
       </c>
       <c r="F86">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G86" s="1">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H86" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I86" s="1">
         <v>149</v>
@@ -4247,11 +4268,11 @@
       </c>
       <c r="L86" t="str">
         <f t="shared" si="5"/>
-        <v>50,80,115,149</v>
+        <v>49,80,114,149</v>
       </c>
       <c r="M86" t="str">
         <f t="shared" si="6"/>
-        <v>60,89,123,157</v>
+        <v>59,88,122,157</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
@@ -4259,7 +4280,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-09_122228_120923_15C_A1B1A4B4A5B5_cory_A_converted.csv</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="11" t="s">
         <v>96</v>
       </c>
       <c r="C87" s="1">
@@ -4299,140 +4320,160 @@
         <v>58,88,121,156</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A88" t="str">
+    <row r="88" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="14" t="str">
         <f t="shared" si="4"/>
         <v>2023-12-08_164634_120823_15C_nononoB2A3B3_tile_B_converted.csv</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C88" s="16">
         <v>45</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D88" s="17">
         <v>55</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="14">
         <v>85</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="14">
         <v>97</v>
       </c>
-      <c r="K88">
+      <c r="G88" s="16"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="16"/>
+      <c r="J88" s="17"/>
+      <c r="K88" s="14">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="L88" t="str">
+      <c r="L88" s="14" t="str">
         <f t="shared" si="5"/>
         <v>45,85</v>
       </c>
-      <c r="M88" t="str">
+      <c r="M88" s="14" t="str">
         <f t="shared" si="6"/>
         <v>55,97</v>
       </c>
     </row>
-    <row r="89" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" t="str">
+    <row r="89" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="10" t="str">
         <f t="shared" si="4"/>
         <v>2023-12-08_164634_120823_15C_nononoB2A3B3_tile_A_converted.csv</v>
       </c>
-      <c r="B89" s="10" t="s">
+      <c r="B89" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C89" s="11">
+      <c r="C89" s="8">
         <v>85</v>
       </c>
-      <c r="D89" s="12">
+      <c r="D89" s="9">
         <v>96</v>
       </c>
-      <c r="G89" s="11"/>
-      <c r="H89" s="12"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="12"/>
-      <c r="K89">
+      <c r="G89" s="8"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="9"/>
+      <c r="K89" s="10">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="L89" t="str">
+      <c r="L89" s="10" t="str">
         <f t="shared" si="5"/>
         <v>85</v>
       </c>
-      <c r="M89" t="str">
+      <c r="M89" s="10" t="str">
         <f t="shared" si="6"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A90" t="str">
+      <c r="N89" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="14" t="str">
         <f t="shared" si="4"/>
         <v>2023-12-08_115055_120823_15C_nononoB2A3B3_cory_B_converted.csv</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C90" s="16">
         <v>46</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="17">
         <v>62</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="14">
         <v>88</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="14">
         <v>96</v>
       </c>
-      <c r="K90">
+      <c r="G90" s="16">
+        <v>121</v>
+      </c>
+      <c r="H90" s="17">
+        <v>131</v>
+      </c>
+      <c r="I90" s="16"/>
+      <c r="J90" s="17"/>
+      <c r="K90" s="14">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="L90" t="str">
+        <v>3</v>
+      </c>
+      <c r="L90" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>46,88</v>
-      </c>
-      <c r="M90" t="str">
+        <v>46,88,121</v>
+      </c>
+      <c r="M90" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>62,96</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A91" t="str">
+        <v>62,96,131</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="10" t="str">
         <f t="shared" si="4"/>
         <v>2023-12-08_115055_120823_15C_nononoB2A3B3_cory_A_converted.csv</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C91" s="1">
+      <c r="C91" s="8">
         <v>50</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="9">
         <v>70</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="10">
         <v>89</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="10">
         <v>105</v>
       </c>
-      <c r="G91" s="1">
+      <c r="G91" s="8">
         <v>127</v>
       </c>
-      <c r="H91" s="2">
+      <c r="H91" s="9">
         <v>137</v>
       </c>
-      <c r="K91">
+      <c r="I91" s="8"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="10">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="L91" t="str">
+      <c r="L91" s="10" t="str">
         <f t="shared" si="5"/>
         <v>50,89,127</v>
       </c>
-      <c r="M91" t="str">
+      <c r="M91" s="10" t="str">
         <f t="shared" si="6"/>
         <v>70,105,137</v>
+      </c>
+      <c r="N91" s="10" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -4440,7 +4481,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-06_152338_120623_23C_B12A13emptyx2_tile_A_converted.csv</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="11" t="s">
         <v>101</v>
       </c>
       <c r="C92" s="1">
@@ -4479,7 +4520,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-06_120950_120623_23C_B12A13emptyx2_cory_A_converted.csv</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="11" t="s">
         <v>102</v>
       </c>
       <c r="C93" s="1">
@@ -4524,7 +4565,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-05_135013_120523_23C_E11A15B15E15_tile_A_converted.csv</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="11" t="s">
         <v>103</v>
       </c>
       <c r="C94" s="1">
@@ -4572,7 +4613,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-05_102008_120523_23C_E11A15B15E15_cory_A_converted.csv</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="11" t="s">
         <v>104</v>
       </c>
       <c r="C95" s="1">
@@ -4617,7 +4658,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-04_141507_120423_23C_E11E12E13E14_tile_A_converted.csv</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="11" t="s">
         <v>105</v>
       </c>
       <c r="C96" s="1">
@@ -4650,7 +4691,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-04_102332_120423_23C_E11E12E13E14_cory_A_converted.csv</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="11" t="s">
         <v>106</v>
       </c>
       <c r="C97" s="1">
@@ -4695,7 +4736,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-03_204617_120323_23C_B11B12B13B14_tile_A_converted.csv</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="11" t="s">
         <v>107</v>
       </c>
       <c r="C98" s="1">
@@ -4722,14 +4763,14 @@
         <f t="shared" si="4"/>
         <v>2023-12-03_171728_120323_23C_B11B12B13B14_cory_A_converted.csv</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="11" t="s">
         <v>108</v>
       </c>
       <c r="C99" s="1">
         <v>52</v>
       </c>
       <c r="D99" s="2">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E99">
         <v>105</v>
@@ -4753,7 +4794,7 @@
       </c>
       <c r="M99" t="str">
         <f t="shared" si="6"/>
-        <v>71,117,155</v>
+        <v>68,117,155</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
@@ -4761,7 +4802,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-03_153050_120323_23C_A11A12A13A14_tile_A_converted.csv</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="11" t="s">
         <v>109</v>
       </c>
       <c r="C100" s="1">
@@ -4794,7 +4835,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-03_114711_120323_23C_A11A12A13A14_cory_A_converted.csv</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="11" t="s">
         <v>110</v>
       </c>
       <c r="C101" s="1">
@@ -4833,7 +4874,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-02_212638_120223_19C_A6A7nono_tile_A_converted.csv</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C102" s="1">
@@ -4860,7 +4901,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-02_180301_120223_19C_A6A7nono_cory_A_converted.csv</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="11" t="s">
         <v>112</v>
       </c>
       <c r="C103" s="1">
@@ -4905,7 +4946,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-02_161820_120223_19C_A6A8A9A10_tile_A_converted.csv</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="11" t="s">
         <v>113</v>
       </c>
       <c r="C104" s="1">
@@ -4938,7 +4979,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-02_125229_120223_19C_A6A8A9A10_cory_A_converted.csv</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="11" t="s">
         <v>114</v>
       </c>
       <c r="C105" s="1">
@@ -4983,7 +5024,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-01_211453_120123_19C_B6B10E8E10_tile_A_converted.csv</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="11" t="s">
         <v>115</v>
       </c>
       <c r="C106" s="1">
@@ -5022,7 +5063,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-01_174656_120123_19C_B6B10E8E10_cory_A_converted.csv</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="11" t="s">
         <v>116</v>
       </c>
       <c r="C107" s="1">
@@ -5067,7 +5108,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-01_155951_120123_19C_E6E7E8E9_tile_A_converted.csv</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" s="11" t="s">
         <v>117</v>
       </c>
       <c r="C108" s="1">
@@ -5106,7 +5147,7 @@
         <f t="shared" si="4"/>
         <v>2023-12-01_122755_120123_19C_E6E7E8E9_cory_A_converted.csv</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B109" s="11" t="s">
         <v>118</v>
       </c>
       <c r="C109" s="1">
@@ -5151,7 +5192,7 @@
         <f t="shared" si="4"/>
         <v>2023-11-30_155822_113023_19C_B6B7B8B9_tile_A_converted.csv</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B110" s="11" t="s">
         <v>119</v>
       </c>
       <c r="C110" s="1">
@@ -5190,7 +5231,7 @@
         <f t="shared" si="4"/>
         <v>2023-11-30_122141_113023_19C_B6B7B8B9_cory_A_converted.csv</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B111" s="11" t="s">
         <v>120</v>
       </c>
       <c r="C111" s="1">

</xml_diff>